<commit_message>
Finally solved them all
</commit_message>
<xml_diff>
--- a/Des-17/hallvard/Sporingshjelp.xlsx
+++ b/Des-17/hallvard/Sporingshjelp.xlsx
@@ -1497,8 +1497,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004BC8473C9FB6814E9B8473C7A7B7C619" ma:contentTypeVersion="11" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="31dfc7d75d7a6c21afec26c44ea2ee81">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d0b67a2-5182-45a4-8314-d1ebde5cd722" xmlns:ns3="2e264c67-d8e6-4443-9155-74276ca7005a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cc62e1d87f2a728355260bb195453de" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004BC8473C9FB6814E9B8473C7A7B7C619" ma:contentTypeVersion="14" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="99fcd28bbefd905546990f28c5c27e15">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d0b67a2-5182-45a4-8314-d1ebde5cd722" xmlns:ns3="2e264c67-d8e6-4443-9155-74276ca7005a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3119bc9265b5691c89f3ede05dc1209d" ns2:_="" ns3:_="">
     <xsd:import namespace="2d0b67a2-5182-45a4-8314-d1ebde5cd722"/>
     <xsd:import namespace="2e264c67-d8e6-4443-9155-74276ca7005a"/>
     <xsd:element name="properties">
@@ -1518,6 +1518,8 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1575,6 +1577,13 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildemerkelapper" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="9b0cd0cd-59ce-4f67-9130-b535f36a0165" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2e264c67-d8e6-4443-9155-74276ca7005a" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1604,6 +1613,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{da1ee6e7-2ebf-4625-9efa-70e2de1e8365}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="2e264c67-d8e6-4443-9155-74276ca7005a">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -1716,12 +1736,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="2e264c67-d8e6-4443-9155-74276ca7005a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2d0b67a2-5182-45a4-8314-d1ebde5cd722">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82375326-A3DC-4620-A289-31858AF2EF1A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E15DDC1-A163-42CA-85A7-18A9E29A6101}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>